<commit_message>
expense page and blob data download gateway added
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,18 +415,62 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>food</v>
+        <v>Cafe</v>
       </c>
       <c r="B2">
-        <v>8000</v>
+        <v>500</v>
       </c>
       <c r="C2" t="str">
-        <v>1/2/2025</v>
+        <v>22/5/2025</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>movie</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3" t="str">
+        <v>16/5/2025</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>travel</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4" t="str">
+        <v>15/5/2025</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>clothing</v>
+      </c>
+      <c r="B5">
+        <v>16000</v>
+      </c>
+      <c r="C5" t="str">
+        <v>14/5/2025</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>rent</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>10/5/2025</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the expense link bug
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,62 +415,73 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Cafe</v>
+        <v>Party</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="C2" t="str">
-        <v>22/5/2025</v>
+        <v>28/5/2025</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>movie</v>
+        <v>Cafe</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C3" t="str">
-        <v>16/5/2025</v>
+        <v>22/5/2025</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>travel</v>
+        <v>movie</v>
       </c>
       <c r="B4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="C4" t="str">
-        <v>15/5/2025</v>
+        <v>16/5/2025</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>clothing</v>
+        <v>travel</v>
       </c>
       <c r="B5">
-        <v>16000</v>
+        <v>3000</v>
       </c>
       <c r="C5" t="str">
-        <v>14/5/2025</v>
+        <v>15/5/2025</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>clothing</v>
+      </c>
+      <c r="B6">
+        <v>16000</v>
+      </c>
+      <c r="C6" t="str">
+        <v>14/5/2025</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>rent</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>10000</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C7" t="str">
         <v>10/5/2025</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>